<commit_message>
[Project] TB-ETF [What] 1. config.py: add taiex, exchange rate, pattern features. 2. main_process.py: add sine wave test data for model verification, corr_mat for data analysis, and modify output pkl file name. 3. nm_features.py: add MinMax mode and TA feature Nm switch. 4. ud_features.py: fix bug: shift label data 1 day. 5. ta_features.py: delete unnecessary import module.
</commit_message>
<xml_diff>
--- a/ta_feature_list.xlsx
+++ b/ta_feature_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="571">
   <si>
     <t>Overlap Studies</t>
   </si>
@@ -1579,6 +1579,250 @@
   </si>
   <si>
     <t>HT_TRENDLINE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL2CROWS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pattern Recognition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL3BLACKCROWS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL3LINESTRIKE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL3OUTSIDE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL3STARSINSOUTH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDL3WHITESOLDIERS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLABANDONEDBABY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLADVANCEBLOCK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLBELTHOLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLBREAKAWAY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLCLOSINGMARUBOZU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLCONCEALBABYSWALL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLCOUNTERATTACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLDARKCLOUDCOVER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLDOJI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLDOJISTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLDRAGONFLYDOJI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLENGULFING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLEVENINGDOJISTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLEVENINGSTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLGAPSIDESIDEWHITE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLGRAVESTONEDOJI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHAMMER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHANGINGMAN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHARAMI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHARAMICROSS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHIGHWAVE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHIKKAKE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHIKKAKEMOD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLHOMINGPIGEON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLIDENTICAL3CROWS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLINNECK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLINVERTEDHAMMER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLKICKING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLKICKINGBYLENGTH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLLADDERBOTTOM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLLONGLEGGEDDOJI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLLONGLINE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLMARUBOZU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLMATCHINGLOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLMATHOLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLMORNINGDOJISTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLMORNINGSTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLONNECK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLPIERCING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLRICKSHAWMAN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLRISEFALL3METHODS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSEPARATINGLINES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSHOOTINGSTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSHORTLINE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSPINNINGTOP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSTALLEDPATTERN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLSTICKSANDWICH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLTAKURI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLTASUKIGAP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLTHRUSTING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLTRISTAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLUNIQUE3RIVER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLUPSIDEGAP2CROWS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDLXSIDEGAP3METHODS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1587,9 +1831,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1614,8 +1858,17 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1640,6 +1893,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1655,14 +1926,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -1678,6 +1949,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4420,7 +4700,7 @@
         <v xml:space="preserve">BETA </v>
       </c>
       <c r="D132" t="str">
-        <f t="shared" ref="D131:D168" si="5">TRIM(B132)</f>
+        <f t="shared" ref="D132:D168" si="5">TRIM(B132)</f>
         <v>BETA</v>
       </c>
       <c r="J132" t="s">
@@ -5111,7 +5391,7 @@
   <dimension ref="A1:C168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5329,13 +5609,13 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -5354,31 +5634,31 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -5469,40 +5749,40 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C45" s="3"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C46" s="3"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -5546,13 +5826,13 @@
       <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
@@ -5689,7 +5969,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>66</v>
+        <v>511</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>218</v>
@@ -5697,553 +5977,553 @@
       <c r="C69" s="7"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="B70" s="7" t="s">
+      <c r="A70" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B70" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="C70" s="7"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="B71" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C71" s="7"/>
+      <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C72" s="7"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="B73" s="7" t="s">
+      <c r="A73" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C73" s="7"/>
+      <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B74" s="7" t="s">
+      <c r="A74" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="B74" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="7"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="B75" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="C75" s="7"/>
+      <c r="C75" s="10"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="B76" s="7" t="s">
+      <c r="A76" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="B76" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C76" s="7"/>
+      <c r="C76" s="10"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="B77" s="7" t="s">
+      <c r="A77" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="B77" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="C77" s="7"/>
+      <c r="C77" s="10"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="B78" s="7" t="s">
+      <c r="A78" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B78" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C78" s="7"/>
+      <c r="C78" s="10"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="B79" s="7" t="s">
+      <c r="A79" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="B79" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C79" s="7"/>
+      <c r="C79" s="10"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="B80" s="7" t="s">
+      <c r="A80" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="B80" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C80" s="7"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="B81" s="7" t="s">
+      <c r="A81" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="B81" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C81" s="7"/>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="B82" s="7" t="s">
+      <c r="A82" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="B82" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C82" s="7"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="B83" s="7" t="s">
+      <c r="A83" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="B83" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C83" s="7"/>
+      <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="A84" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="B84" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C84" s="7"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="A85" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="B85" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C85" s="7"/>
+      <c r="C85" s="10"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="B86" s="7" t="s">
+      <c r="A86" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="B86" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C86" s="7"/>
+      <c r="C86" s="10"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="B87" s="7" t="s">
+      <c r="A87" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="B87" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C87" s="7"/>
+      <c r="C87" s="10"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="B88" s="7" t="s">
+      <c r="A88" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="B88" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C88" s="7"/>
+      <c r="C88" s="10"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="A89" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="C89" s="7"/>
+      <c r="C89" s="10"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="B90" s="7" t="s">
+      <c r="A90" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="C90" s="7"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="B91" s="7" t="s">
+      <c r="A91" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C91" s="7"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="B92" s="7" t="s">
+      <c r="A92" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="B92" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C92" s="7"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="B93" s="7" t="s">
+      <c r="A93" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="B93" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C93" s="7"/>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="B94" s="7" t="s">
+      <c r="A94" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="B94" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="C94" s="7"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="B95" s="7" t="s">
+      <c r="A95" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C95" s="7"/>
+      <c r="C95" s="10"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="B96" s="7" t="s">
+      <c r="A96" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="B96" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="C96" s="7"/>
+      <c r="C96" s="10"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="B97" s="7" t="s">
+      <c r="A97" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="B97" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C97" s="7"/>
+      <c r="C97" s="10"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="B98" s="7" t="s">
+      <c r="A98" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="B98" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="C98" s="7"/>
+      <c r="C98" s="10"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="B99" s="7" t="s">
+      <c r="A99" s="10" t="s">
+        <v>539</v>
+      </c>
+      <c r="B99" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="7"/>
+      <c r="C99" s="10"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="B100" s="7" t="s">
+      <c r="A100" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="B100" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="C100" s="7"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B101" s="7" t="s">
+      <c r="A101" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C101" s="7"/>
+      <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="B102" s="7" t="s">
+      <c r="A102" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="B102" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C102" s="7"/>
+      <c r="C102" s="9"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="B103" s="7" t="s">
+      <c r="A103" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="B103" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="C103" s="7"/>
+      <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="B104" s="7" t="s">
+      <c r="A104" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="B104" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C104" s="7"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B105" s="7" t="s">
+      <c r="A105" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="B105" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C105" s="7"/>
+      <c r="C105" s="10"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="B106" s="7" t="s">
+      <c r="A106" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="B106" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="C106" s="7"/>
+      <c r="C106" s="10"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="B107" s="7" t="s">
+      <c r="A107" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="B107" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="C107" s="7"/>
+      <c r="C107" s="10"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="B108" s="7" t="s">
+      <c r="A108" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="C108" s="7"/>
+      <c r="C108" s="10"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="B109" s="7" t="s">
+      <c r="A109" s="10" t="s">
+        <v>549</v>
+      </c>
+      <c r="B109" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C109" s="7"/>
+      <c r="C109" s="10"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="B110" s="7" t="s">
+      <c r="A110" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="B110" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="C110" s="7"/>
+      <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="B111" s="7" t="s">
+      <c r="A111" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="B111" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C111" s="7"/>
+      <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="B112" s="7" t="s">
+      <c r="A112" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="B112" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C112" s="7"/>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="B113" s="7" t="s">
+      <c r="A113" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C113" s="7"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="B114" s="7" t="s">
+      <c r="A114" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="B114" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="C114" s="7"/>
+      <c r="C114" s="9"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="B115" s="7" t="s">
+      <c r="A115" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="B115" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C115" s="7"/>
+      <c r="C115" s="10"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="B116" s="7" t="s">
+      <c r="A116" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="B116" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="C116" s="7"/>
+      <c r="C116" s="10"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="B117" s="7" t="s">
+      <c r="A117" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="B117" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C117" s="7"/>
+      <c r="C117" s="10"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="B118" s="7" t="s">
+      <c r="A118" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="B118" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="C118" s="7"/>
+      <c r="C118" s="10"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="B119" s="7" t="s">
+      <c r="A119" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="B119" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C119" s="7"/>
+      <c r="C119" s="10"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="B120" s="7" t="s">
+      <c r="A120" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="B120" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="C120" s="7"/>
+      <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="B121" s="7" t="s">
+      <c r="A121" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="B121" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C121" s="7"/>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="B122" s="7" t="s">
+      <c r="A122" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="B122" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="C122" s="7"/>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="B123" s="7" t="s">
+      <c r="A123" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="B123" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C123" s="7"/>
+      <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="B124" s="7" t="s">
+      <c r="A124" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C124" s="7"/>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="B125" s="7" t="s">
+      <c r="A125" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="B125" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="C125" s="7"/>
+      <c r="C125" s="10"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="B126" s="7" t="s">
+      <c r="A126" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="B126" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C126" s="7"/>
+      <c r="C126" s="10"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="B127" s="7" t="s">
+      <c r="A127" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B127" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C127" s="7"/>
+      <c r="C127" s="10"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="B128" s="7" t="s">
+      <c r="A128" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="B128" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C128" s="7"/>
+      <c r="C128" s="10"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="B129" s="7" t="s">
+      <c r="A129" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="B129" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="C129" s="7"/>
+      <c r="C129" s="10"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="B130" s="7" t="s">
+      <c r="A130" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="B130" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="C130" s="7"/>
+      <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
@@ -6590,5 +6870,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>